<commit_message>
Edited the dashboard and coded to show the counts of Colors, Hobbies, and Course
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="166">
   <si>
     <t>Name</t>
   </si>
@@ -621,7 +621,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -645,6 +645,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
@@ -655,7 +697,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="62"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -676,7 +718,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="20"/>
+    <cellStyle name="Hyperlink" xfId="62"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2016,7 +2058,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9DE811-B72B-451C-B73B-4D5CBE41E77C}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="G7" sqref="G7"/>
@@ -3273,6 +3315,48 @@
       </c>
       <c r="D89" s="9">
         <v>45776.684884259259</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15">
+      <c r="A90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90" s="9">
+        <v>45779</v>
+      </c>
+      <c r="D90" s="9">
+        <v>45779.819120370368</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15">
+      <c r="A91" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" s="9">
+        <v>45779</v>
+      </c>
+      <c r="D91" s="9">
+        <v>45779.821006944447</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>48</v>
+      </c>
+      <c r="C92" s="9">
+        <v>45779</v>
+      </c>
+      <c r="D92" s="9">
+        <v>45779.844282407408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify the login code
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>Spire.XLS for .NET</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> logged in</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="455">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -645,6 +648,384 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -711,7 +1092,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="76"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="454"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -732,7 +1113,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="76"/>
+    <cellStyle name="Hyperlink" xfId="454"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1623,7 +2004,7 @@
         <v>100</v>
       </c>
       <c r="M12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15">
@@ -2072,7 +2453,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9DE811-B72B-451C-B73B-4D5CBE41E77C}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="G7" sqref="G7"/>
@@ -3385,6 +3766,341 @@
       </c>
       <c r="D93" s="9">
         <v>45782.677662037</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C94" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D94" s="9">
+        <v>45782.678287037</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15">
+      <c r="A95" t="s">
+        <v>17</v>
+      </c>
+      <c r="B95" t="s">
+        <v>48</v>
+      </c>
+      <c r="C95" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D95" s="9">
+        <v>45782.6805671296</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" ht="15">
+      <c r="B96" t="s">
+        <v>166</v>
+      </c>
+      <c r="C96" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D96" s="9">
+        <v>45782.6814814815</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" ht="15">
+      <c r="B97" t="s">
+        <v>166</v>
+      </c>
+      <c r="C97" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D97" s="9">
+        <v>45782.6815740741</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" ht="15">
+      <c r="B98" t="s">
+        <v>166</v>
+      </c>
+      <c r="C98" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D98" s="9">
+        <v>45782.6871875</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99" t="s">
+        <v>48</v>
+      </c>
+      <c r="C99" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D99" s="9">
+        <v>45782.6889814815</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>48</v>
+      </c>
+      <c r="C100" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D100" s="9">
+        <v>45782.6890162037</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15">
+      <c r="A101" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101" t="s">
+        <v>48</v>
+      </c>
+      <c r="C101" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D101" s="9">
+        <v>45782.6890277778</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15">
+      <c r="A102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B102" t="s">
+        <v>48</v>
+      </c>
+      <c r="C102" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D102" s="9">
+        <v>45782.6890277778</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" t="s">
+        <v>48</v>
+      </c>
+      <c r="C103" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D103" s="9">
+        <v>45782.6890393518</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15">
+      <c r="A104" t="s">
+        <v>17</v>
+      </c>
+      <c r="B104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C104" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D104" s="9">
+        <v>45782.6890393518</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15">
+      <c r="A105" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105" t="s">
+        <v>48</v>
+      </c>
+      <c r="C105" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D105" s="9">
+        <v>45782.6890393518</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15">
+      <c r="A106" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106" t="s">
+        <v>48</v>
+      </c>
+      <c r="C106" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D106" s="9">
+        <v>45782.6890393518</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15">
+      <c r="A107" t="s">
+        <v>17</v>
+      </c>
+      <c r="B107" t="s">
+        <v>48</v>
+      </c>
+      <c r="C107" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D107" s="9">
+        <v>45782.6890509259</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15">
+      <c r="A108" t="s">
+        <v>17</v>
+      </c>
+      <c r="B108" t="s">
+        <v>48</v>
+      </c>
+      <c r="C108" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D108" s="9">
+        <v>45782.6890509259</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15">
+      <c r="A109" t="s">
+        <v>17</v>
+      </c>
+      <c r="B109" t="s">
+        <v>48</v>
+      </c>
+      <c r="C109" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D109" s="9">
+        <v>45782.6890509259</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" ht="15">
+      <c r="B110" t="s">
+        <v>166</v>
+      </c>
+      <c r="C110" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D110" s="9">
+        <v>45782.689537037</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" ht="15">
+      <c r="B111" t="s">
+        <v>166</v>
+      </c>
+      <c r="C111" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D111" s="9">
+        <v>45782.6899189815</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15">
+      <c r="A112" t="s">
+        <v>17</v>
+      </c>
+      <c r="B112" t="s">
+        <v>48</v>
+      </c>
+      <c r="C112" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D112" s="9">
+        <v>45782.6925810185</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15">
+      <c r="A113" t="s">
+        <v>17</v>
+      </c>
+      <c r="B113" t="s">
+        <v>48</v>
+      </c>
+      <c r="C113" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D113" s="9">
+        <v>45782.6937731481</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15">
+      <c r="A114" t="s">
+        <v>17</v>
+      </c>
+      <c r="B114" t="s">
+        <v>48</v>
+      </c>
+      <c r="C114" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D114" s="9">
+        <v>45782.6947106481</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15">
+      <c r="A115" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>48</v>
+      </c>
+      <c r="C115" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D115" s="9">
+        <v>45782.6952893518</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15">
+      <c r="A116" t="s">
+        <v>17</v>
+      </c>
+      <c r="B116" t="s">
+        <v>48</v>
+      </c>
+      <c r="C116" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D116" s="9">
+        <v>45782.6959027778</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15">
+      <c r="A117" t="s">
+        <v>17</v>
+      </c>
+      <c r="B117" t="s">
+        <v>48</v>
+      </c>
+      <c r="C117" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D117" s="9">
+        <v>45782.69625</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15">
+      <c r="A118" t="s">
+        <v>17</v>
+      </c>
+      <c r="B118" t="s">
+        <v>48</v>
+      </c>
+      <c r="C118" s="9">
+        <v>45782</v>
+      </c>
+      <c r="D118" s="9">
+        <v>45782.6970138889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the login code and created a new folder for storing the pictures
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -624,7 +624,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="455">
+  <cellStyleXfs count="469">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -648,6 +648,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1092,7 +1106,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="454"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="468"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1113,7 +1127,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="454"/>
+    <cellStyle name="Hyperlink" xfId="468"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2453,7 +2467,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9DE811-B72B-451C-B73B-4D5CBE41E77C}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="G7" sqref="G7"/>
@@ -4101,6 +4115,20 @@
       </c>
       <c r="D118" s="9">
         <v>45782.6970138889</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15">
+      <c r="A119" t="s">
+        <v>17</v>
+      </c>
+      <c r="B119" t="s">
+        <v>48</v>
+      </c>
+      <c r="C119" s="9">
+        <v>45783</v>
+      </c>
+      <c r="D119" s="9">
+        <v>45783.6893865741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uninstall/reinstall freespire and change the paths
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -624,7 +624,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="469">
+  <cellStyleXfs count="483">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -648,6 +648,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1106,7 +1120,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="468"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="482"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1127,7 +1141,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="468"/>
+    <cellStyle name="Hyperlink" xfId="482"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2467,7 +2481,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9DE811-B72B-451C-B73B-4D5CBE41E77C}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="G7" sqref="G7"/>
@@ -4129,6 +4143,20 @@
       </c>
       <c r="D119" s="9">
         <v>45783.6893865741</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15">
+      <c r="A120" t="s">
+        <v>39</v>
+      </c>
+      <c r="B120" t="s">
+        <v>55</v>
+      </c>
+      <c r="C120" s="9">
+        <v>45783</v>
+      </c>
+      <c r="D120" s="9">
+        <v>45783.7988888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to modify the login code and created a folder for storing the pictures
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="65416" yWindow="65416" windowWidth="21840" windowHeight="13740" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="65416" yWindow="65416" windowWidth="21840" windowHeight="13740" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames/>
   <calcPr calcId="191029"/>
   <extLst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t xml:space="preserve"> logged in</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>C:\Users\Computer\Desktop\EVENTDRIVEN\sint\EVENTDRIVE_ALEGADO\Pictures</t>
   </si>
 </sst>
 </file>
@@ -624,7 +630,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="483">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -648,471 +654,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1120,7 +664,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="482"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1129,10 +673,9 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0"/>
@@ -1141,7 +684,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="482"/>
+    <cellStyle name="Hyperlink" xfId="20"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1520,30 +1063,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86908638-053D-4436-911E-FEB42C1EF90C}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="F1">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultColWidthPt="48" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28125" widthPt="75" style="0" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.00390625" widthPt="42" style="0" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" widthPt="119.25" style="0" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.00390625" widthPt="73.5" style="0" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.57421875" widthPt="39.75" style="0" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.421875" widthPt="107.25" style="0" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.28125" widthPt="132.75" style="0" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28125" widthPt="59.25" style="0" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" widthPt="56.25" style="0" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.421875" widthPt="23.25" style="0" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.00390625" widthPt="57.75" style="0" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" widthPt="69" style="0" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28125" widthPt="54" style="0" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" widthPt="63.75" style="0" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28125" widthPt="106.5" style="0" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.57421875" widthPt="71.25" style="0" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" widthPt="119.25" style="0" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28125" widthPt="43.5" style="0" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.00390625" widthPt="115.5" style="0" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" widthPt="37.5" style="0" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.421875" widthPt="33.75" style="0" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="75.28125" widthPt="395.25" style="0" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15">
+    <row r="1" spans="1:14" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1583,8 +1127,11 @@
       <c r="M1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15">
+      <c r="N1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1623,6 +1170,9 @@
       </c>
       <c r="M2">
         <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15">
@@ -1867,7 +1417,7 @@
       <c r="L8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8">
         <v>1</v>
       </c>
     </row>
@@ -1908,7 +1458,7 @@
       <c r="L9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9">
         <v>1</v>
       </c>
     </row>
@@ -1949,7 +1499,7 @@
       <c r="L10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10">
         <v>1</v>
       </c>
     </row>
@@ -1990,7 +1540,7 @@
       <c r="L11" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11">
         <v>0</v>
       </c>
     </row>
@@ -2031,7 +1581,7 @@
       <c r="L12" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12">
         <v>0</v>
       </c>
     </row>
@@ -2072,7 +1622,7 @@
       <c r="L13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13">
         <v>0</v>
       </c>
     </row>
@@ -2113,7 +1663,7 @@
       <c r="L14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14">
         <v>0</v>
       </c>
     </row>
@@ -2154,7 +1704,7 @@
       <c r="L15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15">
         <v>0</v>
       </c>
     </row>
@@ -2195,7 +1745,7 @@
       <c r="L16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16">
         <v>1</v>
       </c>
     </row>
@@ -2236,7 +1786,7 @@
       <c r="L17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M17">
         <v>1</v>
       </c>
     </row>
@@ -2277,7 +1827,7 @@
       <c r="L18" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18">
         <v>0</v>
       </c>
     </row>
@@ -2318,7 +1868,7 @@
       <c r="L19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M19" s="8">
+      <c r="M19">
         <v>1</v>
       </c>
     </row>
@@ -2359,7 +1909,7 @@
       <c r="L20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="8">
+      <c r="M20">
         <v>0</v>
       </c>
     </row>
@@ -2400,7 +1950,7 @@
       <c r="L21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M21" s="8">
+      <c r="M21">
         <v>1</v>
       </c>
     </row>
@@ -2441,7 +1991,7 @@
       <c r="L22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M22" s="8">
+      <c r="M22">
         <v>1</v>
       </c>
     </row>
@@ -2481,7 +2031,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9DE811-B72B-451C-B73B-4D5CBE41E77C}">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="G7" sqref="G7"/>
@@ -3733,10 +3283,10 @@
       <c r="B89" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="9">
+      <c r="C89" s="4">
         <v>45776</v>
       </c>
-      <c r="D89" s="9">
+      <c r="D89" s="4">
         <v>45776.6848842593</v>
       </c>
     </row>
@@ -3747,10 +3297,10 @@
       <c r="B90" t="s">
         <v>48</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="4">
         <v>45779</v>
       </c>
-      <c r="D90" s="9">
+      <c r="D90" s="4">
         <v>45779.8191203704</v>
       </c>
     </row>
@@ -3761,10 +3311,10 @@
       <c r="B91" t="s">
         <v>55</v>
       </c>
-      <c r="C91" s="9">
+      <c r="C91" s="4">
         <v>45779</v>
       </c>
-      <c r="D91" s="9">
+      <c r="D91" s="4">
         <v>45779.8210069444</v>
       </c>
     </row>
@@ -3775,10 +3325,10 @@
       <c r="B92" t="s">
         <v>48</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C92" s="4">
         <v>45779</v>
       </c>
-      <c r="D92" s="9">
+      <c r="D92" s="4">
         <v>45779.8442824074</v>
       </c>
     </row>
@@ -3789,10 +3339,10 @@
       <c r="B93" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="4">
         <v>45782</v>
       </c>
-      <c r="D93" s="9">
+      <c r="D93" s="4">
         <v>45782.677662037</v>
       </c>
     </row>
@@ -3803,10 +3353,10 @@
       <c r="B94" t="s">
         <v>48</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="4">
         <v>45782</v>
       </c>
-      <c r="D94" s="9">
+      <c r="D94" s="4">
         <v>45782.678287037</v>
       </c>
     </row>
@@ -3817,10 +3367,10 @@
       <c r="B95" t="s">
         <v>48</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="4">
         <v>45782</v>
       </c>
-      <c r="D95" s="9">
+      <c r="D95" s="4">
         <v>45782.6805671296</v>
       </c>
     </row>
@@ -3828,10 +3378,10 @@
       <c r="B96" t="s">
         <v>166</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C96" s="4">
         <v>45782</v>
       </c>
-      <c r="D96" s="9">
+      <c r="D96" s="4">
         <v>45782.6814814815</v>
       </c>
     </row>
@@ -3839,10 +3389,10 @@
       <c r="B97" t="s">
         <v>166</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="4">
         <v>45782</v>
       </c>
-      <c r="D97" s="9">
+      <c r="D97" s="4">
         <v>45782.6815740741</v>
       </c>
     </row>
@@ -3850,10 +3400,10 @@
       <c r="B98" t="s">
         <v>166</v>
       </c>
-      <c r="C98" s="9">
+      <c r="C98" s="4">
         <v>45782</v>
       </c>
-      <c r="D98" s="9">
+      <c r="D98" s="4">
         <v>45782.6871875</v>
       </c>
     </row>
@@ -3864,10 +3414,10 @@
       <c r="B99" t="s">
         <v>48</v>
       </c>
-      <c r="C99" s="9">
+      <c r="C99" s="4">
         <v>45782</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D99" s="4">
         <v>45782.6889814815</v>
       </c>
     </row>
@@ -3878,10 +3428,10 @@
       <c r="B100" t="s">
         <v>48</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="4">
         <v>45782</v>
       </c>
-      <c r="D100" s="9">
+      <c r="D100" s="4">
         <v>45782.6890162037</v>
       </c>
     </row>
@@ -3892,10 +3442,10 @@
       <c r="B101" t="s">
         <v>48</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C101" s="4">
         <v>45782</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D101" s="4">
         <v>45782.6890277778</v>
       </c>
     </row>
@@ -3906,10 +3456,10 @@
       <c r="B102" t="s">
         <v>48</v>
       </c>
-      <c r="C102" s="9">
+      <c r="C102" s="4">
         <v>45782</v>
       </c>
-      <c r="D102" s="9">
+      <c r="D102" s="4">
         <v>45782.6890277778</v>
       </c>
     </row>
@@ -3920,10 +3470,10 @@
       <c r="B103" t="s">
         <v>48</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C103" s="4">
         <v>45782</v>
       </c>
-      <c r="D103" s="9">
+      <c r="D103" s="4">
         <v>45782.6890393518</v>
       </c>
     </row>
@@ -3934,10 +3484,10 @@
       <c r="B104" t="s">
         <v>48</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="4">
         <v>45782</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D104" s="4">
         <v>45782.6890393518</v>
       </c>
     </row>
@@ -3948,10 +3498,10 @@
       <c r="B105" t="s">
         <v>48</v>
       </c>
-      <c r="C105" s="9">
+      <c r="C105" s="4">
         <v>45782</v>
       </c>
-      <c r="D105" s="9">
+      <c r="D105" s="4">
         <v>45782.6890393518</v>
       </c>
     </row>
@@ -3962,10 +3512,10 @@
       <c r="B106" t="s">
         <v>48</v>
       </c>
-      <c r="C106" s="9">
+      <c r="C106" s="4">
         <v>45782</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D106" s="4">
         <v>45782.6890393518</v>
       </c>
     </row>
@@ -3976,10 +3526,10 @@
       <c r="B107" t="s">
         <v>48</v>
       </c>
-      <c r="C107" s="9">
+      <c r="C107" s="4">
         <v>45782</v>
       </c>
-      <c r="D107" s="9">
+      <c r="D107" s="4">
         <v>45782.6890509259</v>
       </c>
     </row>
@@ -3990,10 +3540,10 @@
       <c r="B108" t="s">
         <v>48</v>
       </c>
-      <c r="C108" s="9">
+      <c r="C108" s="4">
         <v>45782</v>
       </c>
-      <c r="D108" s="9">
+      <c r="D108" s="4">
         <v>45782.6890509259</v>
       </c>
     </row>
@@ -4004,10 +3554,10 @@
       <c r="B109" t="s">
         <v>48</v>
       </c>
-      <c r="C109" s="9">
+      <c r="C109" s="4">
         <v>45782</v>
       </c>
-      <c r="D109" s="9">
+      <c r="D109" s="4">
         <v>45782.6890509259</v>
       </c>
     </row>
@@ -4015,10 +3565,10 @@
       <c r="B110" t="s">
         <v>166</v>
       </c>
-      <c r="C110" s="9">
+      <c r="C110" s="4">
         <v>45782</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D110" s="4">
         <v>45782.689537037</v>
       </c>
     </row>
@@ -4026,10 +3576,10 @@
       <c r="B111" t="s">
         <v>166</v>
       </c>
-      <c r="C111" s="9">
+      <c r="C111" s="4">
         <v>45782</v>
       </c>
-      <c r="D111" s="9">
+      <c r="D111" s="4">
         <v>45782.6899189815</v>
       </c>
     </row>
@@ -4040,10 +3590,10 @@
       <c r="B112" t="s">
         <v>48</v>
       </c>
-      <c r="C112" s="9">
+      <c r="C112" s="4">
         <v>45782</v>
       </c>
-      <c r="D112" s="9">
+      <c r="D112" s="4">
         <v>45782.6925810185</v>
       </c>
     </row>
@@ -4054,10 +3604,10 @@
       <c r="B113" t="s">
         <v>48</v>
       </c>
-      <c r="C113" s="9">
+      <c r="C113" s="4">
         <v>45782</v>
       </c>
-      <c r="D113" s="9">
+      <c r="D113" s="4">
         <v>45782.6937731481</v>
       </c>
     </row>
@@ -4068,10 +3618,10 @@
       <c r="B114" t="s">
         <v>48</v>
       </c>
-      <c r="C114" s="9">
+      <c r="C114" s="4">
         <v>45782</v>
       </c>
-      <c r="D114" s="9">
+      <c r="D114" s="4">
         <v>45782.6947106481</v>
       </c>
     </row>
@@ -4082,10 +3632,10 @@
       <c r="B115" t="s">
         <v>48</v>
       </c>
-      <c r="C115" s="9">
+      <c r="C115" s="4">
         <v>45782</v>
       </c>
-      <c r="D115" s="9">
+      <c r="D115" s="4">
         <v>45782.6952893518</v>
       </c>
     </row>
@@ -4096,10 +3646,10 @@
       <c r="B116" t="s">
         <v>48</v>
       </c>
-      <c r="C116" s="9">
+      <c r="C116" s="4">
         <v>45782</v>
       </c>
-      <c r="D116" s="9">
+      <c r="D116" s="4">
         <v>45782.6959027778</v>
       </c>
     </row>
@@ -4110,10 +3660,10 @@
       <c r="B117" t="s">
         <v>48</v>
       </c>
-      <c r="C117" s="9">
+      <c r="C117" s="4">
         <v>45782</v>
       </c>
-      <c r="D117" s="9">
+      <c r="D117" s="4">
         <v>45782.69625</v>
       </c>
     </row>
@@ -4124,10 +3674,10 @@
       <c r="B118" t="s">
         <v>48</v>
       </c>
-      <c r="C118" s="9">
+      <c r="C118" s="4">
         <v>45782</v>
       </c>
-      <c r="D118" s="9">
+      <c r="D118" s="4">
         <v>45782.6970138889</v>
       </c>
     </row>
@@ -4138,10 +3688,10 @@
       <c r="B119" t="s">
         <v>48</v>
       </c>
-      <c r="C119" s="9">
+      <c r="C119" s="4">
         <v>45783</v>
       </c>
-      <c r="D119" s="9">
+      <c r="D119" s="4">
         <v>45783.6893865741</v>
       </c>
     </row>
@@ -4152,11 +3702,25 @@
       <c r="B120" t="s">
         <v>55</v>
       </c>
-      <c r="C120" s="9">
+      <c r="C120" s="4">
         <v>45783</v>
       </c>
-      <c r="D120" s="9">
+      <c r="D120" s="4">
         <v>45783.7988888889</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15">
+      <c r="A121" t="s">
+        <v>17</v>
+      </c>
+      <c r="B121" t="s">
+        <v>48</v>
+      </c>
+      <c r="C121" s="10">
+        <v>45783</v>
+      </c>
+      <c r="D121" s="10">
+        <v>45783.8140277778</v>
       </c>
     </row>
   </sheetData>
@@ -4167,20 +3731,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28125" defaultColWidthPt="48.75" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" ht="15">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="2" ht="15">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4190,7 +3754,7 @@
       </c>
     </row>
     <row r="5" ht="15">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4200,7 +3764,7 @@
       </c>
     </row>
     <row r="8" ht="15">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4210,13 +3774,13 @@
       </c>
     </row>
     <row r="11" ht="15">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="9" t="s">
         <v>158</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://www.e-iceblue.com"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.e-iceblue.com/"/>
     <hyperlink ref="B8" r:id="rId2" display="mailto:support@e-iceblue.com"/>
     <hyperlink ref="B11" r:id="rId3" display="https://www.e-iceblue.com/Buy/Spire.XLS.html"/>
   </hyperlinks>

</xml_diff>

<commit_message>
checked if the update button works
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -630,7 +630,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -654,6 +654,34 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
@@ -664,7 +692,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -684,7 +712,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="20"/>
+    <cellStyle name="Hyperlink" xfId="48"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2031,7 +2059,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9DE811-B72B-451C-B73B-4D5CBE41E77C}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="G7" sqref="G7"/>
@@ -3721,6 +3749,34 @@
       </c>
       <c r="D121" s="10">
         <v>45783.8140277778</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15">
+      <c r="A122" t="s">
+        <v>39</v>
+      </c>
+      <c r="B122" t="s">
+        <v>55</v>
+      </c>
+      <c r="C122" s="10">
+        <v>45783</v>
+      </c>
+      <c r="D122" s="10">
+        <v>45783.8516203704</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15">
+      <c r="A123" t="s">
+        <v>17</v>
+      </c>
+      <c r="B123" t="s">
+        <v>48</v>
+      </c>
+      <c r="C123" s="10">
+        <v>45783</v>
+      </c>
+      <c r="D123" s="10">
+        <v>45783.8556134259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified the login code
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -630,7 +630,7 @@
       <bottom/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -654,6 +654,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -692,7 +762,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="118"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -712,7 +782,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="48"/>
+    <cellStyle name="Hyperlink" xfId="118"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2059,7 +2129,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9DE811-B72B-451C-B73B-4D5CBE41E77C}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="G7" sqref="G7"/>
@@ -3777,6 +3847,76 @@
       </c>
       <c r="D123" s="10">
         <v>45783.8556134259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15">
+      <c r="A124" t="s">
+        <v>17</v>
+      </c>
+      <c r="B124" t="s">
+        <v>48</v>
+      </c>
+      <c r="C124" s="10">
+        <v>45787</v>
+      </c>
+      <c r="D124" s="10">
+        <v>45787.746875</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15">
+      <c r="A125" t="s">
+        <v>17</v>
+      </c>
+      <c r="B125" t="s">
+        <v>48</v>
+      </c>
+      <c r="C125" s="10">
+        <v>45787</v>
+      </c>
+      <c r="D125" s="10">
+        <v>45787.748912037</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15">
+      <c r="A126" t="s">
+        <v>17</v>
+      </c>
+      <c r="B126" t="s">
+        <v>48</v>
+      </c>
+      <c r="C126" s="10">
+        <v>45788</v>
+      </c>
+      <c r="D126" s="10">
+        <v>45788.8391782407</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15">
+      <c r="A127" t="s">
+        <v>17</v>
+      </c>
+      <c r="B127" t="s">
+        <v>48</v>
+      </c>
+      <c r="C127" s="10">
+        <v>45788</v>
+      </c>
+      <c r="D127" s="10">
+        <v>45788.8397222222</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15">
+      <c r="A128" t="s">
+        <v>17</v>
+      </c>
+      <c r="B128" t="s">
+        <v>48</v>
+      </c>
+      <c r="C128" s="10">
+        <v>45788</v>
+      </c>
+      <c r="D128" s="10">
+        <v>45788.8403356481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the update function
</commit_message>
<xml_diff>
--- a/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
+++ b/EVENTDRIVE_ALEGADO/BOOKDB.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="170">
   <si>
     <t>Age</t>
   </si>
@@ -601,7 +601,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="427">
+  <cellStyleXfs count="511">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -625,6 +625,90 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1039,7 +1123,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="426"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="510"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1052,7 +1136,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="426"/>
+    <cellStyle name="Hyperlink" xfId="510"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2428,7 +2512,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B6D9DD-F468-446C-9A12-12FC2CA86E12}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="E9" sqref="E9"/>
@@ -2842,6 +2926,90 @@
         <v>45789.8202314815</v>
       </c>
     </row>
+    <row r="30" spans="1:4" ht="15">
+      <c r="A30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="5">
+        <v>45789</v>
+      </c>
+      <c r="D30" s="5">
+        <v>45789.8446643518</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15">
+      <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="5">
+        <v>45789</v>
+      </c>
+      <c r="D31" s="5">
+        <v>45789.8475578704</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15">
+      <c r="A32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="5">
+        <v>45789</v>
+      </c>
+      <c r="D32" s="5">
+        <v>45789.8509259259</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="5">
+        <v>45789</v>
+      </c>
+      <c r="D33" s="5">
+        <v>45789.8518865741</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="5">
+        <v>45789</v>
+      </c>
+      <c r="D34" s="5">
+        <v>45789.8534027778</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15">
+      <c r="A35" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" t="s">
+        <v>169</v>
+      </c>
+      <c r="C35" s="5">
+        <v>45789</v>
+      </c>
+      <c r="D35" s="5">
+        <v>45789.8743865741</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>